<commit_message>
Update error key to contain more informative diagnostic messages.
</commit_message>
<xml_diff>
--- a/Agents/PassiveAFDD/passiveafdd/sample_data/error_key.xlsx
+++ b/Agents/PassiveAFDD/passiveafdd/sample_data/error_key.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="24" windowWidth="22020" windowHeight="11640"/>
+    <workbookView xWindow="90" yWindow="30" windowWidth="22020" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>Diagnostic</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Unit is off (No Fault)</t>
   </si>
   <si>
-    <t>AFDD-3 (Unit Economizing When it Should)</t>
-  </si>
-  <si>
     <t>Damper should be at minimum position but is not (Fault)</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>Insufficient outdoor-air intake (Fault)</t>
   </si>
   <si>
-    <t>Damper is not at minimum when is should not be (Fault)</t>
-  </si>
-  <si>
     <t>AFDD-6 (Schedule)</t>
   </si>
   <si>
@@ -120,7 +114,46 @@
     <t>Missing data necessary for fault detection</t>
   </si>
   <si>
-    <t>AFDD-2 (Unit Economizing When it Should)</t>
+    <t>AFDD-3 (Unit Economizing When it Should Not)</t>
+  </si>
+  <si>
+    <t>AFDD-2 (Unit Not Economizing When it Should)</t>
+  </si>
+  <si>
+    <t>Mixed-air temperature (MAT) is not trended and the heating or cooling is active.  Since discharge-air temperature (DAT) is used instead of MAT the heating and cooling cannot be active (unfavorable condition).</t>
+  </si>
+  <si>
+    <t>The passive diagnostic does not deterimine which temperature sensor is faulty.</t>
+  </si>
+  <si>
+    <t>Unit is not fully utilizing economzing or a mechanical issue is causing outdoor-air fraction to be too low.</t>
+  </si>
+  <si>
+    <t>OAF calculation is not in the range of [0,1.25]</t>
+  </si>
+  <si>
+    <t>Since some units utilize integrated economizer logic and only the compressor command is known a unit maybe in a cooling mode and economizing when the compressor is off.</t>
+  </si>
+  <si>
+    <t>Missing outdoor-air tempeature, return-air temperature, mixed-air temperature, outdoor damper command, or compressor command.</t>
+  </si>
+  <si>
+    <t>The difference of the outdoor-air temperature and mixed-air temperature should be at least 5F for OAF calculation.</t>
+  </si>
+  <si>
+    <t>Damper is not at minimum when is  not be (Fault)</t>
+  </si>
+  <si>
+    <t>Outdoor-air damper is significantly above the minimum (correct for current conditions) command.</t>
+  </si>
+  <si>
+    <t>Missing supply-fan status, outdoor-air tempeature, return-air temperature, mixed-air temperature, outdoor damper command, or compressor command.</t>
+  </si>
+  <si>
+    <t>Missing supply-fan status, outdoor-air temperature, mixed-air temperature, or return-air temperature sensor readings.</t>
+  </si>
+  <si>
+    <t>Note</t>
   </si>
 </sst>
 </file>
@@ -497,27 +530,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C54"/>
+  <dimension ref="B2:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="82.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -525,7 +564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>20</v>
       </c>
@@ -533,15 +572,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>21</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>22</v>
       </c>
@@ -549,7 +591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>23</v>
       </c>
@@ -557,7 +599,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>24</v>
       </c>
@@ -565,7 +607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>25</v>
       </c>
@@ -573,15 +615,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>27</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>29</v>
       </c>
@@ -589,12 +634,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>30</v>
       </c>
@@ -602,7 +647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>31</v>
       </c>
@@ -610,15 +655,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
         <v>32</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>33</v>
       </c>
@@ -626,31 +674,40 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>36</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
         <v>37</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B21" s="4">
         <v>38</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
         <v>39</v>
       </c>
@@ -658,12 +715,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
         <v>40</v>
       </c>
@@ -671,31 +728,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B26" s="4">
         <v>41</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B27" s="4">
         <v>43</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B28" s="4">
         <v>47</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B29" s="4">
         <v>49</v>
       </c>
@@ -703,12 +766,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B32" s="4">
         <v>50</v>
       </c>
@@ -716,55 +779,64 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B33" s="4">
         <v>51</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B34" s="4">
         <v>52</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B35" s="4">
         <v>53</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B36" s="4">
         <v>56</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="D36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B37" s="4">
         <v>57</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="4">
         <v>58</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="D38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="4">
         <v>59</v>
       </c>
@@ -772,12 +844,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C41" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="4">
         <v>60</v>
       </c>
@@ -785,55 +857,70 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="4">
         <v>61</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="4">
         <v>62</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="D44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="4">
         <v>63</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="4">
         <v>66</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="D46" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="4">
         <v>67</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="4">
         <v>68</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="D48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="4">
         <v>69</v>
       </c>
@@ -841,33 +928,33 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C51" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="4">
         <v>70</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="4">
         <v>71</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="4">
         <v>77</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -881,7 +968,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -893,7 +980,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>